<commit_message>
L2 Update BVA and BBT-TC. Rename the display name of the test cases to reflect the docs
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79540380-803F-4D51-906F-90206AF9365B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39933D8-FE32-4BE1-BA8F-B41BB090A81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="702" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="702" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="121">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -296,24 +296,6 @@
     <t>output data</t>
   </si>
   <si>
-    <t>titlu</t>
-  </si>
-  <si>
-    <t>regizor</t>
-  </si>
-  <si>
-    <t>an aparitie</t>
-  </si>
-  <si>
-    <t>actori</t>
-  </si>
-  <si>
-    <t>categorie</t>
-  </si>
-  <si>
-    <t>cuvinte cheie</t>
-  </si>
-  <si>
     <t>expected</t>
   </si>
   <si>
@@ -366,6 +348,12 @@
   </si>
   <si>
     <t>F01</t>
+  </si>
+  <si>
+    <t>TC1_ECP</t>
+  </si>
+  <si>
+    <t>TC3_BVA</t>
   </si>
   <si>
     <t>Statistics</t>
@@ -623,6 +611,12 @@
   </si>
   <si>
     <t>TC4</t>
+  </si>
+  <si>
+    <t>TC2_ECP</t>
+  </si>
+  <si>
+    <t>TC8_BVA</t>
   </si>
 </sst>
 </file>
@@ -846,7 +840,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1043,19 +1037,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1281,7 +1262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1452,86 +1433,77 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1549,10 +1521,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1562,48 +1534,29 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1962,7 +1915,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J4" s="33">
         <v>234</v>
@@ -1973,7 +1926,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J5" s="33">
         <v>234</v>
@@ -1985,7 +1938,7 @@
         <v>7</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J6" s="33">
         <v>234</v>
@@ -2147,7 +2100,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="I9" sqref="I9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2176,7 +2129,7 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="49" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C3" s="50"/>
       <c r="D3" s="50"/>
@@ -2191,14 +2144,14 @@
       <c r="C5" s="52"/>
       <c r="D5" s="52"/>
       <c r="E5" s="52"/>
-      <c r="G5" s="99" t="s">
+      <c r="G5" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
     </row>
     <row r="6" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
@@ -2224,7 +2177,7 @@
       </c>
       <c r="J6" s="46"/>
       <c r="K6" s="42"/>
-      <c r="L6" s="98" t="s">
+      <c r="L6" s="95" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2233,25 +2186,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="60" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E7" s="4"/>
       <c r="G7" s="54"/>
       <c r="H7" s="44"/>
       <c r="I7" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L7" s="98" t="s">
-        <v>38</v>
+        <v>79</v>
+      </c>
+      <c r="K7" s="106" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="95" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -2261,13 +2214,13 @@
       <c r="C8" s="61"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I8" s="2">
         <v>3</v>
@@ -2276,10 +2229,10 @@
         <v>40</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="L8" s="97" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="L8" s="94" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2289,13 +2242,13 @@
       <c r="C9" s="62"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G9" s="10">
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I9" s="2">
         <v>2</v>
@@ -2304,10 +2257,10 @@
         <v>-10</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L9" s="97" t="s">
-        <v>102</v>
+        <v>83</v>
+      </c>
+      <c r="L9" s="94" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -2315,17 +2268,17 @@
         <v>4</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="G10" s="93">
+      <c r="G10" s="90">
         <v>3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I10" s="16">
         <v>-1</v>
@@ -2334,10 +2287,10 @@
         <v>20000.5</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="L10" s="101" t="s">
-        <v>103</v>
+        <v>82</v>
+      </c>
+      <c r="L10" s="98" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2347,13 +2300,13 @@
       <c r="C11" s="59"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="93">
+        <v>75</v>
+      </c>
+      <c r="G11" s="90">
         <v>4</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I11" s="16">
         <v>10</v>
@@ -2362,10 +2315,10 @@
         <v>50.99</v>
       </c>
       <c r="K11" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="98" t="s">
         <v>87</v>
-      </c>
-      <c r="L11" s="101" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
@@ -2375,36 +2328,36 @@
       <c r="C12" s="48"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="93">
+        <v>73</v>
+      </c>
+      <c r="G12" s="90">
         <v>5</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="101"/>
+      <c r="L12" s="98"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>7</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="G13" s="93">
+      <c r="G13" s="90">
         <v>6</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
-      <c r="L13" s="101"/>
+      <c r="L13" s="98"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
@@ -2413,34 +2366,34 @@
       <c r="C14" s="48"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="93">
+        <v>34</v>
+      </c>
+      <c r="G14" s="90">
         <v>7</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
-      <c r="L14" s="101"/>
+      <c r="L14" s="98"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>9</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="G15" s="93">
+      <c r="G15" s="90">
         <v>8</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
-      <c r="L15" s="101"/>
+      <c r="L15" s="98"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
@@ -2454,14 +2407,14 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
-      <c r="L16" s="101"/>
+      <c r="L16" s="98"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>11</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -2470,7 +2423,7 @@
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
-      <c r="L17" s="101"/>
+      <c r="L17" s="98"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
@@ -2484,14 +2437,14 @@
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
-      <c r="L18" s="101"/>
+      <c r="L18" s="98"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>13</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2500,7 +2453,7 @@
       <c r="I19" s="16"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
-      <c r="L19" s="101"/>
+      <c r="L19" s="98"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
@@ -2512,7 +2465,7 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F22" s="40"/>
       <c r="G22" s="40"/>
@@ -2545,8 +2498,8 @@
   </sheetPr>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2578,8 +2531,8 @@
       <c r="E1" s="38"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="118" t="s">
-        <v>95</v>
+      <c r="B3" s="104" t="s">
+        <v>91</v>
       </c>
       <c r="C3" s="50"/>
       <c r="D3" s="50"/>
@@ -2589,51 +2542,51 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="58" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C5" s="58"/>
       <c r="D5" s="58"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="94" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="95"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="95"/>
-      <c r="N5" s="96"/>
+      <c r="G5" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="93"/>
     </row>
     <row r="6" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E6" s="6"/>
       <c r="G6" s="53" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I6" s="53" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J6" s="43" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K6" s="55" t="s">
         <v>30</v>
       </c>
       <c r="L6" s="56"/>
       <c r="M6" s="56"/>
-      <c r="N6" s="119" t="s">
+      <c r="N6" s="105" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2642,10 +2595,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2655,38 +2608,38 @@
       <c r="I7" s="54"/>
       <c r="J7" s="44"/>
       <c r="K7" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="N7" s="98" t="s">
-        <v>48</v>
+        <v>80</v>
+      </c>
+      <c r="N7" s="95" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="59"/>
       <c r="C8" s="61"/>
       <c r="D8" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
-      <c r="G8" s="93">
+      <c r="G8" s="90">
         <v>1</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K8" s="8">
         <v>1</v>
@@ -2695,32 +2648,32 @@
         <v>0.01</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="59"/>
       <c r="C9" s="61"/>
       <c r="D9" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E9">
         <v>3</v>
       </c>
-      <c r="G9" s="93">
+      <c r="G9" s="90">
         <v>2</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>119</v>
-      </c>
       <c r="J9" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K9" s="8">
         <v>2</v>
@@ -2729,32 +2682,32 @@
         <v>1</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="59"/>
       <c r="C10" s="61"/>
       <c r="D10" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
-      <c r="G10" s="93">
+      <c r="G10" s="90">
         <v>3</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K10" s="8">
         <v>7</v>
@@ -2763,32 +2716,32 @@
         <v>9999.99</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="59"/>
       <c r="C11" s="61"/>
       <c r="D11" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
-      <c r="G11" s="93">
+      <c r="G11" s="90">
         <v>4</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K11" s="8">
         <v>8</v>
@@ -2797,32 +2750,32 @@
         <v>10000</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="48"/>
       <c r="C12" s="62"/>
       <c r="D12" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E12">
         <v>6</v>
       </c>
-      <c r="G12" s="93">
+      <c r="G12" s="90">
         <v>5</v>
       </c>
       <c r="H12" s="8">
         <v>7</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K12" s="8">
         <v>5</v>
@@ -2831,10 +2784,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -2842,25 +2795,25 @@
         <v>2</v>
       </c>
       <c r="C13" s="60" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E13">
         <v>7</v>
       </c>
-      <c r="G13" s="93">
+      <c r="G13" s="90">
         <v>6</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K13" s="8">
         <v>9</v>
@@ -2869,17 +2822,17 @@
         <v>10000.01</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="59"/>
       <c r="C14" s="61"/>
       <c r="D14" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E14">
         <v>8</v>
@@ -2888,13 +2841,13 @@
         <v>7</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K14" s="8">
         <v>0</v>
@@ -2903,17 +2856,17 @@
         <v>0</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="59"/>
       <c r="C15" s="61"/>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E15">
         <v>9</v>
@@ -2925,10 +2878,10 @@
         <v>6</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K15" s="8">
         <v>9</v>
@@ -2937,17 +2890,17 @@
         <v>50</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="59"/>
       <c r="C16" s="61"/>
       <c r="D16" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -2967,7 +2920,7 @@
       <c r="B17" s="59"/>
       <c r="C17" s="61"/>
       <c r="D17" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E17">
         <v>11</v>
@@ -2987,7 +2940,7 @@
       <c r="B18" s="48"/>
       <c r="C18" s="62"/>
       <c r="D18" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E18">
         <v>12</v>
@@ -3008,10 +2961,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E19">
         <v>13</v>
@@ -3031,7 +2984,7 @@
       <c r="B20" s="59"/>
       <c r="C20" s="61"/>
       <c r="D20" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E20">
         <v>14</v>
@@ -3199,8 +3152,8 @@
   </sheetPr>
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3208,8 +3161,8 @@
     <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.77734375" customWidth="1"/>
+    <col min="10" max="10" width="25.77734375" customWidth="1"/>
     <col min="12" max="12" width="9.88671875" customWidth="1"/>
     <col min="13" max="13" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.88671875" customWidth="1"/>
@@ -3224,78 +3177,60 @@
       <c r="E1" s="38"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="92" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
+      <c r="B3" s="107" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="109"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="90" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+      <c r="C4" s="88" t="s">
+        <v>45</v>
       </c>
       <c r="D4" s="76" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F4" s="41" t="s">
         <v>30</v>
       </c>
       <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="45" t="s">
+      <c r="H4" s="42"/>
+      <c r="I4" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="75"/>
-      <c r="C5" s="91"/>
+      <c r="C5" s="89"/>
       <c r="D5" s="77"/>
-      <c r="E5" s="89"/>
+      <c r="E5" s="87"/>
       <c r="F5" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="J5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" s="87" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="88"/>
-      <c r="M5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -3303,19 +3238,27 @@
         <v>1</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="102"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="106"/>
-      <c r="M6" s="104"/>
-      <c r="N6" s="103"/>
+        <v>49</v>
+      </c>
+      <c r="D6" s="99" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="100"/>
+      <c r="F6" s="4">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <v>40</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="100" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
@@ -3323,17 +3266,25 @@
         <v>2</v>
       </c>
       <c r="C7" s="73"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="93"/>
+      <c r="D7" s="101" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="90"/>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4">
+        <v>-10</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7" s="100" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
@@ -3341,17 +3292,25 @@
         <v>3</v>
       </c>
       <c r="C8" s="73"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="108"/>
-      <c r="K8" s="108"/>
-      <c r="L8" s="108"/>
-      <c r="M8" s="108"/>
-      <c r="N8" s="93"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="90" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="8">
+        <v>7</v>
+      </c>
+      <c r="G8" s="8">
+        <v>9999.99</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="100" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
@@ -3359,17 +3318,25 @@
         <v>4</v>
       </c>
       <c r="C9" s="73"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="93"/>
-      <c r="N9" s="93"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="8">
+        <v>9</v>
+      </c>
+      <c r="G9" s="8">
+        <v>50</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="100" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
@@ -3377,17 +3344,15 @@
         <v>5</v>
       </c>
       <c r="C10" s="73"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="108"/>
-      <c r="K10" s="109"/>
-      <c r="L10" s="110"/>
-      <c r="M10" s="108"/>
-      <c r="N10" s="93"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="100" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
@@ -3395,17 +3360,15 @@
         <v>6</v>
       </c>
       <c r="C11" s="73"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="113"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="108"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="109"/>
-      <c r="L11" s="110"/>
-      <c r="M11" s="108"/>
-      <c r="N11" s="93"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="100" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
@@ -3413,17 +3376,15 @@
         <v>7</v>
       </c>
       <c r="C12" s="73"/>
-      <c r="D12" s="107"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="113"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="108"/>
-      <c r="K12" s="109"/>
-      <c r="L12" s="110"/>
-      <c r="M12" s="108"/>
-      <c r="N12" s="93"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="100" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12">
@@ -3431,17 +3392,15 @@
         <v>8</v>
       </c>
       <c r="C13" s="74"/>
-      <c r="D13" s="114"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="115"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="116"/>
-      <c r="L13" s="117"/>
-      <c r="M13" s="115"/>
-      <c r="N13" s="115"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="100" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
@@ -3460,7 +3419,7 @@
     </row>
     <row r="15" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
@@ -3479,23 +3438,23 @@
     </row>
     <row r="17" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C17" s="66" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="68"/>
       <c r="F17" s="69"/>
       <c r="G17" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H17" s="66" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I17" s="67"/>
       <c r="J17" s="68"/>
       <c r="K17" s="68"/>
       <c r="L17" s="69"/>
       <c r="M17" s="66" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N17" s="67"/>
       <c r="O17" s="68"/>
@@ -3503,47 +3462,47 @@
     </row>
     <row r="18" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="80" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C18" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="H18" s="82" t="s">
         <v>62</v>
-      </c>
-      <c r="E18" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="86" t="s">
-        <v>65</v>
-      </c>
-      <c r="H18" s="82" t="s">
-        <v>66</v>
       </c>
       <c r="I18" s="83"/>
       <c r="J18" s="65" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K18" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="M18" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="L18" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="M18" s="70" t="s">
-        <v>66</v>
-      </c>
       <c r="N18" s="65" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O18" s="65" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P18" s="64" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
@@ -3565,7 +3524,7 @@
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C20" s="19">
         <v>4</v>
@@ -3575,20 +3534,14 @@
       <c r="F20" s="22"/>
       <c r="G20" s="27"/>
       <c r="H20" s="78" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I20" s="79"/>
-      <c r="J20" s="2">
-        <v>3</v>
-      </c>
-      <c r="K20" s="21">
-        <v>3</v>
-      </c>
-      <c r="L20" s="22">
-        <v>0</v>
-      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="22"/>
       <c r="M20" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="21"/>
@@ -3598,21 +3551,13 @@
       <c r="M21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="28">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="F4:H4"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="C6:C13"/>
     <mergeCell ref="B4:B5"/>

</xml_diff>